<commit_message>
Implement header re-initialization feature to allow skipping header rows. Improve tests.
</commit_message>
<xml_diff>
--- a/source/Sylvan.Data.Excel.Tests/Data/SkipHeaders.xlsx
+++ b/source/Sylvan.Data.Excel.Tests/Data/SkipHeaders.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\source\Sylvan.Data.Excel\source\Sylvan.Data.Excel.Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A77BF8E-B0AB-4B62-9328-10746A7901B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D325BDB1-E4C5-4187-AF64-A5C1C95FBD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="735" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Annual Report 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Cookies!" sheetId="2" r:id="rId1"/>
+    <sheet name="Annual Report 2022" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Prepared by Sally in accounting</t>
   </si>
@@ -98,6 +99,30 @@
   </si>
   <si>
     <t>Lippmans, Inc.</t>
+  </si>
+  <si>
+    <t>Fabulous cookie recipe</t>
+  </si>
+  <si>
+    <t>Flour</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>.5lb</t>
+  </si>
+  <si>
+    <t>Eggs</t>
   </si>
 </sst>
 </file>
@@ -437,11 +462,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF75CA7D-6278-4DA6-92D8-05EC9D5CD9FE}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>